<commit_message>
Diagrams tuned. Part IV functions table supplemented.
</commit_message>
<xml_diff>
--- a/EvaluativeCoefficient.xlsx
+++ b/EvaluativeCoefficient.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -88,7 +88,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="uk-UA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -99,6 +99,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -108,13 +112,22 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>TSP</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+          </c:marker>
           <c:trendline>
-            <c:name>Approximation</c:name>
+            <c:spPr>
+              <a:ln w="31750"/>
+            </c:spPr>
             <c:trendlineType val="linear"/>
             <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
@@ -122,8 +135,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="9.4215056707639369E-2"/>
-                  <c:y val="-5.7032089501710619E-2"/>
+                  <c:x val="7.952966276725737E-2"/>
+                  <c:y val="-1.5207106562193788E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -131,6 +144,162 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Estimate!$C$2:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>915118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>689171</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1050601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1235984</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1462809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2388093</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2181190</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3352219</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2470779</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6288111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2225372</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2634595</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3159391</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3484388</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4314186</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4992013</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4443875</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6586402</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7830482</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7523549</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8706230</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9490654</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8521431</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6593880</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11651401</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13435570</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13041890</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>17323695</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17047695</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18508216</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21549903</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18324915</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19280751</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>25118163</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24332493</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>21209859</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>22659498</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>27345299</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>29459034</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>31223365</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>33294720</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>32887993</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>33326640</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>33022262</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>37619034</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>37837451</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>37594079</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42861406</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42328536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Estimate!$B$2:$B$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -281,162 +450,6 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>78946</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Estimate!$C$2:$C$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
-                <c:pt idx="0">
-                  <c:v>915118</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>689171</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1050601</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1235984</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1462809</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2388093</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2181190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3352219</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2470779</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6288111</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2225372</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2634595</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3159391</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3484388</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4314186</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4992013</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4443875</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6586402</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7830482</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7523549</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8706230</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9490654</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8521431</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6593880</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>11651401</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>13435570</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13041890</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>17323695</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>17047695</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>18508216</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>21549903</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>18324915</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>19280751</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>25118163</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>24332493</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>21209859</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>22659498</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>27345299</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>29459034</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>31223365</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>33294720</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>32887993</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>33326640</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>33022262</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>37619034</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>37837451</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>37594079</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>42861406</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>42328536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,11 +464,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63869312"/>
-        <c:axId val="63870848"/>
+        <c:axId val="215229952"/>
+        <c:axId val="215231488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63869312"/>
+        <c:axId val="215229952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,23 +478,35 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63870848"/>
+        <c:crossAx val="215231488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63870848"/>
+        <c:axId val="215231488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                  <a:alpha val="21000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63869312"/>
+        <c:crossAx val="215229952"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -506,7 +531,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="uk-UA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -865,11 +890,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88697088"/>
-        <c:axId val="88711168"/>
+        <c:axId val="215244160"/>
+        <c:axId val="215254144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88697088"/>
+        <c:axId val="215244160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -880,12 +905,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88711168"/>
+        <c:crossAx val="215254144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88711168"/>
+        <c:axId val="215254144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,7 +921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88697088"/>
+        <c:crossAx val="215244160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -921,7 +946,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="uk-UA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -27608,11 +27633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89161728"/>
-        <c:axId val="89163264"/>
+        <c:axId val="215049344"/>
+        <c:axId val="215050880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89161728"/>
+        <c:axId val="215049344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27622,7 +27647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89163264"/>
+        <c:crossAx val="215050880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27630,7 +27655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89163264"/>
+        <c:axId val="215050880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2000"/>
@@ -27642,7 +27667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89161728"/>
+        <c:crossAx val="215049344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27767,9 +27792,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -27807,7 +27832,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -27879,7 +27904,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -28055,8 +28080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28682,8 +28707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4439"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B4439"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>